<commit_message>
Metricas buffer y nobuffer
</commit_message>
<xml_diff>
--- a/Metricas.xlsx
+++ b/Metricas.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/castillo/ATS/Practica/BigData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0069094-67EF-1241-85C6-B668D4AECC7C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{522EEE84-3A64-5D4D-A7A6-41DF4936E69B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="32880" windowHeight="20540" xr2:uid="{F6DBAD19-278F-3745-90B5-20B824FBCE4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>BufferFile</t>
   </si>
@@ -39,52 +39,85 @@
     <t>Ficheros</t>
   </si>
   <si>
-    <t>38 MB</t>
-  </si>
-  <si>
     <t>900 B</t>
   </si>
   <si>
-    <t>77 MB</t>
-  </si>
-  <si>
     <t>NoBufferFIle</t>
   </si>
   <si>
     <t>Tiempos 900 B</t>
   </si>
   <si>
-    <t>Tiempos 38 MB</t>
-  </si>
-  <si>
-    <t>Tiempos 77 MB</t>
-  </si>
-  <si>
-    <t>Tiempos 154 MB</t>
-  </si>
-  <si>
-    <t>153 MB</t>
-  </si>
-  <si>
     <t>NO BUFFERFILE</t>
   </si>
   <si>
     <t>BUFFERFILE</t>
   </si>
   <si>
-    <t>TIEMPOS 38 MB</t>
-  </si>
-  <si>
-    <t>TIEMPOS 77 MB</t>
-  </si>
-  <si>
-    <t>TIEMPOS 154 MB</t>
+    <t>Tiempos 500 KB</t>
+  </si>
+  <si>
+    <t>TIEMPOS 5 KB</t>
+  </si>
+  <si>
+    <t>5 KB</t>
+  </si>
+  <si>
+    <t>500 KB</t>
+  </si>
+  <si>
+    <t>Tiempos 5 MB</t>
+  </si>
+  <si>
+    <t>TIEMPOS 10 MB</t>
+  </si>
+  <si>
+    <t>TIEMPOS 20 MB</t>
+  </si>
+  <si>
+    <t>TIEMPOS 100 MB</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Sample2</t>
+  </si>
+  <si>
+    <t>Sample3</t>
+  </si>
+  <si>
+    <t>Sample4</t>
+  </si>
+  <si>
+    <t>Sample5</t>
+  </si>
+  <si>
+    <t>Sample6</t>
+  </si>
+  <si>
+    <t>Sample7</t>
+  </si>
+  <si>
+    <t>5 MB</t>
+  </si>
+  <si>
+    <t>10 MB</t>
+  </si>
+  <si>
+    <t>20 MB</t>
+  </si>
+  <si>
+    <t>100 MB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -114,10 +147,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -126,9 +162,11 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -154,12 +192,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A080FEFA-4321-8348-9160-83C1BA3358CD}" name="Tabla1" displayName="Tabla1" ref="B8:D12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="B8:D12" xr:uid="{AA7B5AAB-260A-D240-8A03-5E4C5BA15402}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A080FEFA-4321-8348-9160-83C1BA3358CD}" name="Tabla1" displayName="Tabla1" ref="B8:D15" totalsRowShown="0" headerRowDxfId="4" dataDxfId="2">
+  <autoFilter ref="B8:D15" xr:uid="{AA7B5AAB-260A-D240-8A03-5E4C5BA15402}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EC2AF6F5-0D97-A442-9255-539F3C4D15D0}" name="Ficheros" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{C057E112-5963-F447-9656-4985090009C8}" name="NoBufferFIle" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{567D2C6F-3191-4A4F-9725-8CBA1E0A4A76}" name="BufferFile" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{EC2AF6F5-0D97-A442-9255-539F3C4D15D0}" name="Ficheros" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{C057E112-5963-F447-9656-4985090009C8}" name="NoBufferFIle" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{567D2C6F-3191-4A4F-9725-8CBA1E0A4A76}" name="BufferFile" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -462,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519361BC-A214-6B4B-9583-6858A8A58973}">
-  <dimension ref="B6:E35"/>
+  <dimension ref="B6:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,6 +512,10 @@
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
@@ -485,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>0</v>
@@ -493,271 +535,569 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
         <v>1.5E-3</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>1.5E-3</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2">
-        <v>4.66</v>
-      </c>
-      <c r="D10" s="2">
-        <v>2.96</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.8E-3</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>9.2899999999999991</v>
-      </c>
-      <c r="D11" s="2">
-        <v>6.28</v>
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.1128</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7.9000000000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2">
-        <v>21.36</v>
-      </c>
-      <c r="D12" s="2">
-        <v>14.11</v>
+        <v>22</v>
+      </c>
+      <c r="C12" s="3">
+        <f>F26</f>
+        <v>0.77220000000000011</v>
+      </c>
+      <c r="D12" s="3">
+        <f>F35</f>
+        <v>0.51076666666666659</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="3">
+        <f>G26</f>
+        <v>1.5504666666666667</v>
+      </c>
+      <c r="D13" s="3">
+        <f>G35</f>
+        <v>1.0309666666666664</v>
+      </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3">
+        <f>H26</f>
+        <v>3.170666666666667</v>
+      </c>
+      <c r="D14" s="3">
+        <f>H35</f>
+        <v>1.9115666666666666</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3">
+        <f>I26</f>
+        <v>16.203773333333331</v>
+      </c>
+      <c r="D15" s="3">
+        <f>I35</f>
+        <v>10.099266666666667</v>
+      </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="2">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2">
         <v>1E-3</v>
       </c>
-      <c r="C22" s="2">
-        <v>4.6500000000000004</v>
-      </c>
       <c r="D22" s="2">
-        <v>9.69</v>
+        <v>0.02</v>
       </c>
       <c r="E22" s="2">
-        <v>22.27</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="2">
+        <v>0.13439999999999999</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.78420000000000001</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.5449999999999999</v>
+      </c>
+      <c r="H22" s="2">
+        <v>3.2928999999999999</v>
+      </c>
+      <c r="I22" s="2">
+        <v>16.8599</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="C23" s="2">
-        <v>4.63</v>
-      </c>
       <c r="D23" s="2">
-        <v>8.84</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="E23" s="2">
-        <v>21.78</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="2">
+        <v>0.1018</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.77190000000000003</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.544</v>
+      </c>
+      <c r="H23" s="2">
+        <v>3.0684999999999998</v>
+      </c>
+      <c r="I23" s="2">
+        <v>15.965299999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2">
         <v>2E-3</v>
       </c>
-      <c r="C24" s="2">
-        <v>4.6900000000000004</v>
-      </c>
       <c r="D24" s="2">
-        <v>9.33</v>
+        <v>3.8E-3</v>
       </c>
       <c r="E24" s="2">
-        <v>20.04</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+        <v>0.1022</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.76049999999999995</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.5624</v>
+      </c>
+      <c r="H24" s="2">
+        <v>3.1505999999999998</v>
+      </c>
+      <c r="I24" s="2">
+        <v>15.78612</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="2">
-        <f>SUM(B22:B24)/3</f>
-        <v>1.5333333333333334E-3</v>
-      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="2"/>
       <c r="C26" s="2">
         <f>SUM(C22:C24)/3</f>
-        <v>4.6566666666666672</v>
+        <v>1.5333333333333334E-3</v>
       </c>
       <c r="D26" s="2">
         <f>SUM(D22:D24)/3</f>
-        <v>9.2866666666666671</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="E26" s="2">
         <f>SUM(E22:E24)/3</f>
-        <v>21.363333333333333</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+        <v>0.1128</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" ref="F26:I26" si="0">SUM(F22:F24)/3</f>
+        <v>0.77220000000000011</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5504666666666667</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="0"/>
+        <v>3.170666666666667</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>16.203773333333331</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="2">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2">
         <v>1.5E-3</v>
       </c>
-      <c r="C31" s="2">
-        <v>2.99</v>
-      </c>
       <c r="D31" s="2">
-        <v>6.33</v>
+        <v>1.5E-3</v>
       </c>
       <c r="E31" s="2">
-        <v>14.47</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="2">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.51890000000000003</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="I31" s="2">
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2">
         <v>1.8E-3</v>
       </c>
-      <c r="C32" s="2">
-        <v>2.95</v>
-      </c>
       <c r="D32" s="2">
-        <v>6.52</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="E32" s="2">
-        <v>14.11</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="2">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.49980000000000002</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1.8640000000000001</v>
+      </c>
+      <c r="I32" s="2">
+        <v>9.6655999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2">
         <v>1.2899999999999999E-3</v>
       </c>
-      <c r="C33" s="2">
-        <v>2.96</v>
-      </c>
       <c r="D33" s="2">
-        <v>5.99</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="E33" s="2">
-        <v>13.75</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.51359999999999995</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1.0408999999999999</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1.8656999999999999</v>
+      </c>
+      <c r="I33" s="2">
+        <v>9.6821999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="2">
-        <f>SUM(B31:B33)/3</f>
-        <v>1.5300000000000001E-3</v>
-      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="2"/>
       <c r="C35" s="2">
         <f>SUM(C31:C33)/3</f>
-        <v>2.9666666666666668</v>
+        <v>1.5300000000000001E-3</v>
       </c>
       <c r="D35" s="2">
         <f>SUM(D31:D33)/3</f>
-        <v>6.28</v>
+        <v>1.8000000000000002E-3</v>
       </c>
       <c r="E35" s="2">
         <f>SUM(E31:E33)/3</f>
-        <v>14.11</v>
-      </c>
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" ref="F35:I35" si="1">SUM(F31:F33)/3</f>
+        <v>0.51076666666666659</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0309666666666664</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9115666666666666</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>10.099266666666667</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>